<commit_message>
Sorted nodes wrt country
</commit_message>
<xml_diff>
--- a/data/TEx Cartography081116.xlsx
+++ b/data/TEx Cartography081116.xlsx
@@ -5274,6 +5274,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3609975</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>276225</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5543,10 +5591,10 @@
   <dimension ref="A1:Y177"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C170" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U70" sqref="U70"/>
+      <selection pane="bottomRight" activeCell="D154" sqref="D154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1"/>

</xml_diff>